<commit_message>
Remove Zoom link that has no metadata
</commit_message>
<xml_diff>
--- a/resource-data.xlsx
+++ b/resource-data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mazenk/IdeaProjects/BC-CPC-COVID-19-ws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40062A5A-E75E-4942-A2BE-6B2947678B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4AFFF0-7FCC-0945-8D83-8CBE7BEA131A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
     <sheet name="COVID Resources-HCP" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'COVID Resources-HCP'!$A$1:$H$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'COVID Resources-HCP'!$A$1:$H$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'COVID Resources-HCP'!$D$1:$H$20</definedName>
   </definedNames>
   <calcPr calcId="191028" concurrentCalc="0"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="178">
   <si>
     <t>Audience</t>
   </si>
@@ -1282,17 +1282,17 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.453125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="4" width="23.453125" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1374,90 +1374,90 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7"/>
       <c r="C7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8"/>
       <c r="C8" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="16"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="C9" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="16"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10"/>
       <c r="C10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11"/>
       <c r="C11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13"/>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="16"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16"/>
       <c r="D16" s="16"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17"/>
       <c r="D17" s="16"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="16"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D26" s="16"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D27" s="16"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D28" s="16"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D32" s="16"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D38" s="16"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D44" s="16"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D45" s="16"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D46" s="16"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D47" s="16"/>
     </row>
   </sheetData>
@@ -1480,27 +1480,27 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" customWidth="1"/>
-    <col min="4" max="4" width="40.6328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" style="4" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="41.54296875" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="4" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="120.6328125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="22.81640625" customWidth="1"/>
+    <col min="8" max="8" width="120.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="47.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>4</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>12</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>4</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>4</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>4</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>4</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>4</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>12</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>12</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>4</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>4</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>4</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>4</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>4</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>4</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>20</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>4</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>4</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>4</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>12</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>4</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>4</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>4</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>4</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>4</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>4</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>4</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>4</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>4</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>4</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>4</v>
       </c>
@@ -2867,13 +2867,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H57" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:H57" xr:uid="{01F70AC8-F911-4676-9746-6E4145D26250}">
+  <autoFilter ref="A1:H56" xr:uid="{01F70AC8-F911-4676-9746-6E4145D26250}">
     <filterColumn colId="5">
       <filters>
         <filter val="Pallium Canada"/>
@@ -2884,8 +2879,8 @@
         <filter val="Education"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H57">
-      <sortCondition ref="D1:D57"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H56">
+      <sortCondition ref="D1:D56"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H49">
@@ -2948,12 +2943,11 @@
     <hyperlink ref="H6" r:id="rId53" xr:uid="{7C24382D-49F8-4923-91B9-773AC826C128}"/>
     <hyperlink ref="H52" r:id="rId54" xr:uid="{50859075-8410-415E-85F0-9F5C01B1BD02}"/>
     <hyperlink ref="H39" r:id="rId55" xr:uid="{589F1475-1A72-435B-ADD5-CA6EBCBB2C52}"/>
-    <hyperlink ref="H57" r:id="rId56" xr:uid="{B009F998-D90B-4BD6-B959-7FBD4ABD935C}"/>
-    <hyperlink ref="H15" r:id="rId57" xr:uid="{4F1D6A2D-E11C-41B7-B026-66CF7367B005}"/>
+    <hyperlink ref="H15" r:id="rId56" xr:uid="{4F1D6A2D-E11C-41B7-B026-66CF7367B005}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="80" fitToHeight="0" orientation="landscape" r:id="rId58"/>
-  <legacyDrawing r:id="rId59"/>
+  <pageSetup scale="80" fitToHeight="0" orientation="landscape" r:id="rId57"/>
+  <legacyDrawing r:id="rId58"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
@@ -3003,31 +2997,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Progress_x0020_Status xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
-    <y9iw xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
-    <Partner_x0020_References xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
-    <rpgi xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
-    <_x0069_b23 xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
-    <tpcx xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
-    <SharedWithUsers xmlns="311946b4-224d-423c-891c-e94db618f1dc">
-      <UserInfo>
-        <DisplayName>Jing Xu</DisplayName>
-        <AccountId>3676</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Eman Hassan</DisplayName>
-        <AccountId>18</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D83B78EDF08BA4595F0FC8E1D40F77E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d58860e619a0f61508b05be848c722d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="25d400d9-5b28-422d-aa61-69b545335a0f" xmlns:ns3="311946b4-224d-423c-891c-e94db618f1dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05e6d3fea9933738f77cb1eee93e2816" ns2:_="" ns3:_="">
     <xsd:import namespace="25d400d9-5b28-422d-aa61-69b545335a0f"/>
@@ -3287,6 +3256,31 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Progress_x0020_Status xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
+    <y9iw xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
+    <Partner_x0020_References xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
+    <rpgi xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
+    <_x0069_b23 xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
+    <tpcx xmlns="25d400d9-5b28-422d-aa61-69b545335a0f" xsi:nil="true"/>
+    <SharedWithUsers xmlns="311946b4-224d-423c-891c-e94db618f1dc">
+      <UserInfo>
+        <DisplayName>Jing Xu</DisplayName>
+        <AccountId>3676</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Eman Hassan</DisplayName>
+        <AccountId>18</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0389F28-6455-476A-BA68-55D730824EA0}">
   <ds:schemaRefs>
@@ -3296,23 +3290,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D64718D8-AFE2-4E90-AB45-D4C55AF4374A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="311946b4-224d-423c-891c-e94db618f1dc"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="25d400d9-5b28-422d-aa61-69b545335a0f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28CB2480-C82C-4199-9EFA-AE254CDEBB8B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3329,4 +3306,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D64718D8-AFE2-4E90-AB45-D4C55AF4374A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="311946b4-224d-423c-891c-e94db618f1dc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="25d400d9-5b28-422d-aa61-69b545335a0f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>